<commit_message>
Adiciona ramo com gráfico novo
</commit_message>
<xml_diff>
--- a/trabalho_1/Diagramas/Diagrama_gantt.xlsx
+++ b/trabalho_1/Diagramas/Diagrama_gantt.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>Atividade</t>
   </si>
@@ -120,6 +120,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF0000CC"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -130,18 +142,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="mediumGray">
-        <bgColor rgb="FF00B050"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="31">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -426,6 +428,54 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -468,106 +518,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -668,6 +623,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -683,67 +677,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1099,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH35" sqref="AH35"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,36 +1070,36 @@
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="46"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="57"/>
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2"/>
@@ -1806,36 +1758,36 @@
       <c r="A17" s="28"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="45"/>
-      <c r="AA17" s="45"/>
-      <c r="AB17" s="45"/>
-      <c r="AC17" s="45"/>
-      <c r="AD17" s="45"/>
-      <c r="AE17" s="45"/>
-      <c r="AF17" s="46"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
+      <c r="AA17" s="56"/>
+      <c r="AB17" s="56"/>
+      <c r="AC17" s="56"/>
+      <c r="AD17" s="56"/>
+      <c r="AE17" s="56"/>
+      <c r="AF17" s="57"/>
     </row>
     <row r="18" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18"/>
@@ -2338,311 +2290,265 @@
       <c r="AF31" s="27"/>
     </row>
     <row r="32" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
-      <c r="X32" s="35"/>
-      <c r="Y32" s="35"/>
-      <c r="Z32" s="35"/>
-      <c r="AA32" s="35"/>
-      <c r="AB32" s="35"/>
-      <c r="AC32" s="35"/>
-      <c r="AD32" s="35"/>
-      <c r="AE32" s="35"/>
-      <c r="AF32" s="35"/>
-    </row>
-    <row r="33" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E33" s="44" t="s">
+      <c r="E32" s="47"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="48"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="48"/>
+      <c r="T32" s="48"/>
+      <c r="U32" s="48"/>
+      <c r="V32" s="48"/>
+      <c r="W32" s="48"/>
+      <c r="X32" s="48"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="48"/>
+      <c r="AA32" s="48"/>
+      <c r="AB32" s="48"/>
+      <c r="AC32" s="48"/>
+      <c r="AD32" s="48"/>
+      <c r="AE32" s="48"/>
+      <c r="AF32" s="48"/>
+    </row>
+    <row r="33" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="45"/>
-      <c r="U33" s="45"/>
-      <c r="V33" s="45"/>
-      <c r="W33" s="45"/>
-      <c r="X33" s="45"/>
-      <c r="Y33" s="45"/>
-      <c r="Z33" s="45"/>
-      <c r="AA33" s="45"/>
-      <c r="AB33" s="45"/>
-      <c r="AC33" s="45"/>
-      <c r="AD33" s="45"/>
-      <c r="AE33" s="45"/>
-      <c r="AF33" s="46"/>
-    </row>
-    <row r="34" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="56"/>
+      <c r="S33" s="56"/>
+      <c r="T33" s="56"/>
+      <c r="U33" s="56"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="56"/>
+      <c r="X33" s="56"/>
+      <c r="Y33" s="56"/>
+      <c r="Z33" s="56"/>
+      <c r="AA33" s="56"/>
+      <c r="AB33" s="56"/>
+      <c r="AC33" s="56"/>
+      <c r="AD33" s="56"/>
+      <c r="AE33" s="56"/>
+      <c r="AF33" s="57"/>
+    </row>
+    <row r="34" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E35" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F35" s="48">
+      <c r="F35" s="6">
         <v>0</v>
       </c>
-      <c r="G35" s="49">
+      <c r="G35" s="3">
         <v>1</v>
       </c>
-      <c r="H35" s="49">
+      <c r="H35" s="3">
         <v>2</v>
       </c>
-      <c r="I35" s="49">
+      <c r="I35" s="3">
         <v>3</v>
       </c>
-      <c r="J35" s="49">
+      <c r="J35" s="3">
         <v>4</v>
       </c>
-      <c r="K35" s="49">
+      <c r="K35" s="3">
         <v>5</v>
       </c>
-      <c r="L35" s="49">
+      <c r="L35" s="3">
         <v>6</v>
       </c>
-      <c r="M35" s="49">
+      <c r="M35" s="3">
         <v>7</v>
       </c>
-      <c r="N35" s="49">
+      <c r="N35" s="3">
         <v>8</v>
       </c>
-      <c r="O35" s="49">
+      <c r="O35" s="3">
         <v>9</v>
       </c>
-      <c r="P35" s="49">
+      <c r="P35" s="3">
         <v>10</v>
       </c>
-      <c r="Q35" s="49">
+      <c r="Q35" s="3">
         <v>11</v>
       </c>
-      <c r="R35" s="49">
+      <c r="R35" s="3">
         <v>12</v>
       </c>
-      <c r="S35" s="49">
+      <c r="S35" s="3">
         <v>13</v>
       </c>
-      <c r="T35" s="49">
+      <c r="T35" s="3">
         <v>14</v>
       </c>
-      <c r="U35" s="49">
+      <c r="U35" s="3">
         <v>15</v>
       </c>
-      <c r="V35" s="49">
+      <c r="V35" s="3">
         <v>16</v>
       </c>
-      <c r="W35" s="49">
+      <c r="W35" s="3">
         <v>17</v>
       </c>
-      <c r="X35" s="49">
+      <c r="X35" s="3">
         <v>18</v>
       </c>
-      <c r="Y35" s="49">
+      <c r="Y35" s="3">
         <v>19</v>
       </c>
-      <c r="Z35" s="49">
+      <c r="Z35" s="3">
         <v>20</v>
       </c>
-      <c r="AA35" s="49">
+      <c r="AA35" s="3">
         <v>21</v>
       </c>
-      <c r="AB35" s="49">
+      <c r="AB35" s="3">
         <v>22</v>
       </c>
-      <c r="AC35" s="49">
+      <c r="AC35" s="3">
         <v>23</v>
       </c>
-      <c r="AD35" s="49">
+      <c r="AD35" s="3">
         <v>24</v>
       </c>
-      <c r="AE35" s="49">
+      <c r="AE35" s="3">
         <v>25</v>
       </c>
-      <c r="AF35" s="50">
+      <c r="AF35" s="4">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="5:32" x14ac:dyDescent="0.25">
+      <c r="E36" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="8" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="C36" s="8">
+      <c r="F36" s="11"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="12"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="12"/>
+      <c r="AC36" s="12"/>
+      <c r="AD36" s="12"/>
+      <c r="AE36" s="12"/>
+      <c r="AF36" s="13"/>
+    </row>
+    <row r="37" spans="5:32" x14ac:dyDescent="0.25">
+      <c r="E37" s="10">
         <v>0</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="20"/>
+      <c r="AA37" s="20"/>
+      <c r="AB37" s="20"/>
+      <c r="AC37" s="20"/>
+      <c r="AD37" s="20"/>
+      <c r="AE37" s="20"/>
+      <c r="AF37" s="16"/>
+    </row>
+    <row r="38" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="10">
+        <v>1</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="37"/>
+      <c r="AE38" s="20"/>
+      <c r="AF38" s="16"/>
+    </row>
+    <row r="39" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="10">
         <v>3</v>
       </c>
-      <c r="F36" s="52"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="53"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
-      <c r="T36" s="53"/>
-      <c r="U36" s="53"/>
-      <c r="V36" s="53"/>
-      <c r="W36" s="53"/>
-      <c r="X36" s="53"/>
-      <c r="Y36" s="53"/>
-      <c r="Z36" s="53"/>
-      <c r="AA36" s="53"/>
-      <c r="AB36" s="53"/>
-      <c r="AC36" s="53"/>
-      <c r="AD36" s="53"/>
-      <c r="AE36" s="53"/>
-      <c r="AF36" s="54"/>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
-        <v>0</v>
-      </c>
-      <c r="B37" s="20">
-        <v>0</v>
-      </c>
-      <c r="C37" s="20">
-        <v>4</v>
-      </c>
-      <c r="E37" s="33">
-        <v>0</v>
-      </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="37"/>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="37"/>
-      <c r="R37" s="37"/>
-      <c r="S37" s="37"/>
-      <c r="T37" s="37"/>
-      <c r="U37" s="37"/>
-      <c r="V37" s="37"/>
-      <c r="W37" s="37"/>
-      <c r="X37" s="37"/>
-      <c r="Y37" s="37"/>
-      <c r="Z37" s="37"/>
-      <c r="AA37" s="37"/>
-      <c r="AB37" s="37"/>
-      <c r="AC37" s="37"/>
-      <c r="AD37" s="37"/>
-      <c r="AE37" s="37"/>
-      <c r="AF37" s="38"/>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A38" s="14">
-        <v>1</v>
-      </c>
-      <c r="B38" s="20">
-        <v>4</v>
-      </c>
-      <c r="C38" s="20">
-        <v>6</v>
-      </c>
-      <c r="E38" s="33">
-        <v>1</v>
-      </c>
-      <c r="F38" s="55"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="37"/>
-      <c r="Q38" s="37"/>
-      <c r="R38" s="37"/>
-      <c r="S38" s="37"/>
-      <c r="T38" s="37"/>
-      <c r="U38" s="37"/>
-      <c r="V38" s="37"/>
-      <c r="W38" s="37"/>
-      <c r="X38" s="37"/>
-      <c r="Y38" s="37"/>
-      <c r="Z38" s="37"/>
-      <c r="AA38" s="37"/>
-      <c r="AB38" s="37"/>
-      <c r="AC38" s="37"/>
-      <c r="AD38" s="37"/>
-      <c r="AE38" s="37"/>
-      <c r="AF38" s="38"/>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
-        <v>3</v>
-      </c>
-      <c r="B39" s="20">
-        <v>22</v>
-      </c>
-      <c r="C39" s="20">
-        <v>1</v>
-      </c>
-      <c r="E39" s="33">
-        <v>3</v>
-      </c>
-      <c r="F39" s="55"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="37"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
       <c r="Q39" s="37"/>
       <c r="R39" s="37"/>
       <c r="S39" s="37"/>
@@ -2652,316 +2558,243 @@
       <c r="W39" s="37"/>
       <c r="X39" s="37"/>
       <c r="Y39" s="37"/>
-      <c r="Z39" s="37"/>
-      <c r="AA39" s="37"/>
-      <c r="AB39" s="59"/>
-      <c r="AC39" s="37"/>
-      <c r="AD39" s="37"/>
-      <c r="AE39" s="51"/>
-      <c r="AF39" s="38"/>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="34"/>
+      <c r="AD39" s="46"/>
+      <c r="AE39" s="35"/>
+      <c r="AF39" s="16"/>
+    </row>
+    <row r="40" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E40" s="10">
         <v>4</v>
       </c>
-      <c r="B40" s="20">
-        <v>9</v>
-      </c>
-      <c r="C40" s="20">
-        <v>9</v>
-      </c>
-      <c r="E40" s="33">
-        <v>4</v>
-      </c>
-      <c r="F40" s="55"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="37"/>
-      <c r="N40" s="37"/>
-      <c r="O40" s="60"/>
-      <c r="P40" s="60"/>
-      <c r="Q40" s="60"/>
-      <c r="R40" s="60"/>
-      <c r="S40" s="60"/>
-      <c r="T40" s="60"/>
-      <c r="U40" s="60"/>
-      <c r="V40" s="60"/>
-      <c r="W40" s="60"/>
-      <c r="X40" s="37"/>
-      <c r="Y40" s="37"/>
-      <c r="Z40" s="37"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="44"/>
+      <c r="S40" s="44"/>
+      <c r="T40" s="44"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="44"/>
+      <c r="W40" s="44"/>
+      <c r="X40" s="44"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="36"/>
       <c r="AA40" s="37"/>
       <c r="AB40" s="37"/>
       <c r="AC40" s="37"/>
-      <c r="AD40" s="37"/>
-      <c r="AE40" s="37"/>
-      <c r="AF40" s="38"/>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
+      <c r="AD40" s="8"/>
+      <c r="AE40" s="20"/>
+      <c r="AF40" s="16"/>
+    </row>
+    <row r="41" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="10">
         <v>5</v>
       </c>
-      <c r="B41" s="20">
-        <v>18</v>
-      </c>
-      <c r="C41" s="20">
-        <v>4</v>
-      </c>
-      <c r="E41" s="33">
-        <v>5</v>
-      </c>
-      <c r="F41" s="55"/>
+      <c r="F41" s="36"/>
       <c r="G41" s="37"/>
       <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="37"/>
-      <c r="O41" s="37"/>
-      <c r="P41" s="37"/>
-      <c r="Q41" s="37"/>
-      <c r="R41" s="37"/>
-      <c r="S41" s="37"/>
-      <c r="T41" s="37"/>
-      <c r="U41" s="37"/>
-      <c r="V41" s="37"/>
-      <c r="W41" s="37"/>
-      <c r="X41" s="60"/>
-      <c r="Y41" s="60"/>
-      <c r="Z41" s="60"/>
-      <c r="AA41" s="60"/>
-      <c r="AB41" s="37"/>
-      <c r="AC41" s="37"/>
-      <c r="AD41" s="37"/>
-      <c r="AE41" s="37"/>
-      <c r="AF41" s="38"/>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
-        <v>6</v>
-      </c>
-      <c r="B42" s="20">
-        <v>0</v>
-      </c>
-      <c r="C42" s="20">
-        <v>3</v>
-      </c>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="39"/>
+      <c r="Z41" s="43"/>
+      <c r="AA41" s="44"/>
+      <c r="AB41" s="44"/>
+      <c r="AC41" s="45"/>
+      <c r="AD41" s="19"/>
+      <c r="AE41" s="20"/>
+      <c r="AF41" s="16"/>
+    </row>
+    <row r="42" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E42" s="33">
         <v>6</v>
       </c>
-      <c r="F42" s="58"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
       <c r="K42" s="37"/>
       <c r="L42" s="37"/>
       <c r="M42" s="37"/>
       <c r="N42" s="37"/>
       <c r="O42" s="37"/>
       <c r="P42" s="37"/>
-      <c r="Q42" s="37"/>
-      <c r="R42" s="37"/>
-      <c r="S42" s="37"/>
-      <c r="T42" s="37"/>
-      <c r="U42" s="37"/>
-      <c r="V42" s="37"/>
-      <c r="W42" s="37"/>
-      <c r="X42" s="37"/>
-      <c r="Y42" s="37"/>
-      <c r="Z42" s="37"/>
-      <c r="AA42" s="37"/>
-      <c r="AB42" s="37"/>
-      <c r="AC42" s="37"/>
-      <c r="AD42" s="37"/>
-      <c r="AE42" s="37"/>
-      <c r="AF42" s="38"/>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="8"/>
+      <c r="AA42" s="8"/>
+      <c r="AB42" s="8"/>
+      <c r="AC42" s="8"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="20"/>
+      <c r="AF42" s="16"/>
+    </row>
+    <row r="43" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="10">
         <v>7</v>
       </c>
-      <c r="B43" s="20">
-        <v>3</v>
-      </c>
-      <c r="C43" s="20">
-        <v>6</v>
-      </c>
-      <c r="E43" s="33">
-        <v>7</v>
-      </c>
-      <c r="F43" s="55"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="60"/>
-      <c r="J43" s="60"/>
-      <c r="K43" s="60"/>
-      <c r="L43" s="60"/>
-      <c r="M43" s="60"/>
-      <c r="N43" s="60"/>
-      <c r="O43" s="37"/>
-      <c r="P43" s="37"/>
-      <c r="Q43" s="37"/>
-      <c r="R43" s="37"/>
-      <c r="S43" s="37"/>
-      <c r="T43" s="37"/>
-      <c r="U43" s="37"/>
-      <c r="V43" s="37"/>
-      <c r="W43" s="37"/>
-      <c r="X43" s="37"/>
-      <c r="Y43" s="37"/>
-      <c r="Z43" s="37"/>
-      <c r="AA43" s="37"/>
-      <c r="AB43" s="37"/>
-      <c r="AC43" s="37"/>
-      <c r="AD43" s="37"/>
-      <c r="AE43" s="37"/>
-      <c r="AF43" s="38"/>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
+      <c r="F43" s="38"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="20"/>
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="20"/>
+      <c r="AA43" s="20"/>
+      <c r="AB43" s="20"/>
+      <c r="AC43" s="20"/>
+      <c r="AD43" s="20"/>
+      <c r="AE43" s="20"/>
+      <c r="AF43" s="16"/>
+    </row>
+    <row r="44" spans="5:32" x14ac:dyDescent="0.25">
+      <c r="E44" s="10">
         <v>9</v>
       </c>
-      <c r="B44" s="20">
-        <v>18</v>
-      </c>
-      <c r="C44" s="20">
-        <v>2</v>
-      </c>
-      <c r="E44" s="33">
-        <v>9</v>
-      </c>
-      <c r="F44" s="55"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="37"/>
-      <c r="N44" s="37"/>
-      <c r="O44" s="37"/>
-      <c r="P44" s="37"/>
-      <c r="Q44" s="37"/>
-      <c r="R44" s="37"/>
-      <c r="S44" s="37"/>
-      <c r="T44" s="37"/>
-      <c r="U44" s="37"/>
-      <c r="V44" s="37"/>
-      <c r="W44" s="37"/>
-      <c r="X44" s="41"/>
-      <c r="Y44" s="41"/>
-      <c r="Z44" s="37"/>
-      <c r="AA44" s="37"/>
-      <c r="AB44" s="37"/>
-      <c r="AC44" s="37"/>
-      <c r="AD44" s="37"/>
-      <c r="AE44" s="37"/>
-      <c r="AF44" s="38"/>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A45" s="14">
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="18"/>
+      <c r="AA44" s="18"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="20"/>
+      <c r="AF44" s="16"/>
+    </row>
+    <row r="45" spans="5:32" x14ac:dyDescent="0.25">
+      <c r="E45" s="10">
         <v>10</v>
       </c>
-      <c r="B45" s="20">
-        <v>3</v>
-      </c>
-      <c r="C45" s="20">
-        <v>8</v>
-      </c>
-      <c r="E45" s="33">
-        <v>10</v>
-      </c>
-      <c r="F45" s="55"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="41"/>
-      <c r="O45" s="41"/>
-      <c r="P45" s="41"/>
-      <c r="Q45" s="37"/>
-      <c r="R45" s="37"/>
-      <c r="S45" s="37"/>
-      <c r="T45" s="37"/>
-      <c r="U45" s="37"/>
-      <c r="V45" s="37"/>
-      <c r="W45" s="37"/>
-      <c r="X45" s="37"/>
-      <c r="Y45" s="37"/>
-      <c r="Z45" s="37"/>
-      <c r="AA45" s="37"/>
-      <c r="AB45" s="37"/>
-      <c r="AC45" s="37"/>
-      <c r="AD45" s="37"/>
-      <c r="AE45" s="37"/>
-      <c r="AF45" s="38"/>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A46" s="14">
+      <c r="F45" s="19"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="20"/>
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="20"/>
+      <c r="AA45" s="20"/>
+      <c r="AB45" s="20"/>
+      <c r="AC45" s="20"/>
+      <c r="AD45" s="20"/>
+      <c r="AE45" s="20"/>
+      <c r="AF45" s="16"/>
+    </row>
+    <row r="46" spans="5:32" x14ac:dyDescent="0.25">
+      <c r="E46" s="10">
         <v>11</v>
       </c>
-      <c r="B46" s="20">
-        <v>11</v>
-      </c>
-      <c r="C46" s="20">
-        <v>7</v>
-      </c>
-      <c r="E46" s="33">
-        <v>11</v>
-      </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="37"/>
-      <c r="L46" s="37"/>
-      <c r="M46" s="37"/>
-      <c r="N46" s="37"/>
-      <c r="O46" s="37"/>
-      <c r="P46" s="37"/>
-      <c r="Q46" s="41"/>
-      <c r="R46" s="41"/>
-      <c r="S46" s="41"/>
-      <c r="T46" s="41"/>
-      <c r="U46" s="41"/>
-      <c r="V46" s="41"/>
-      <c r="W46" s="41"/>
-      <c r="X46" s="37"/>
-      <c r="Y46" s="37"/>
-      <c r="Z46" s="37"/>
-      <c r="AA46" s="37"/>
-      <c r="AB46" s="37"/>
-      <c r="AC46" s="37"/>
-      <c r="AD46" s="37"/>
-      <c r="AE46" s="37"/>
-      <c r="AF46" s="38"/>
-    </row>
-    <row r="47" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="20"/>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="20"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="18"/>
+      <c r="U46" s="18"/>
+      <c r="V46" s="18"/>
+      <c r="W46" s="18"/>
+      <c r="X46" s="18"/>
+      <c r="Y46" s="18"/>
+      <c r="Z46" s="20"/>
+      <c r="AA46" s="20"/>
+      <c r="AB46" s="20"/>
+      <c r="AC46" s="20"/>
+      <c r="AD46" s="20"/>
+      <c r="AE46" s="20"/>
+      <c r="AF46" s="16"/>
+    </row>
+    <row r="47" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="22" t="str">
-        <f>"-"</f>
-        <v>-</v>
-      </c>
-      <c r="C47" s="22">
-        <v>0</v>
-      </c>
-      <c r="E47" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="56"/>
+      <c r="F47" s="25"/>
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
       <c r="I47" s="26"/>
@@ -2989,38 +2822,38 @@
       <c r="AE47" s="26"/>
       <c r="AF47" s="27"/>
     </row>
-    <row r="48" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="5:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E49" s="44" t="s">
+      <c r="E49" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="45"/>
-      <c r="P49" s="45"/>
-      <c r="Q49" s="45"/>
-      <c r="R49" s="45"/>
-      <c r="S49" s="45"/>
-      <c r="T49" s="45"/>
-      <c r="U49" s="45"/>
-      <c r="V49" s="45"/>
-      <c r="W49" s="45"/>
-      <c r="X49" s="45"/>
-      <c r="Y49" s="45"/>
-      <c r="Z49" s="45"/>
-      <c r="AA49" s="45"/>
-      <c r="AB49" s="45"/>
-      <c r="AC49" s="45"/>
-      <c r="AD49" s="45"/>
-      <c r="AE49" s="45"/>
-      <c r="AF49" s="46"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="56"/>
+      <c r="R49" s="56"/>
+      <c r="S49" s="56"/>
+      <c r="T49" s="56"/>
+      <c r="U49" s="56"/>
+      <c r="V49" s="56"/>
+      <c r="W49" s="56"/>
+      <c r="X49" s="56"/>
+      <c r="Y49" s="56"/>
+      <c r="Z49" s="56"/>
+      <c r="AA49" s="56"/>
+      <c r="AB49" s="56"/>
+      <c r="AC49" s="56"/>
+      <c r="AD49" s="56"/>
+      <c r="AE49" s="56"/>
+      <c r="AF49" s="57"/>
     </row>
     <row r="50" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3172,33 +3005,33 @@
       <c r="E53" s="10">
         <v>0</v>
       </c>
-      <c r="F53" s="39"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="37"/>
-      <c r="M53" s="37"/>
-      <c r="N53" s="37"/>
-      <c r="O53" s="37"/>
-      <c r="P53" s="37"/>
-      <c r="Q53" s="37"/>
-      <c r="R53" s="37"/>
-      <c r="S53" s="37"/>
-      <c r="T53" s="37"/>
-      <c r="U53" s="37"/>
-      <c r="V53" s="37"/>
-      <c r="W53" s="37"/>
-      <c r="X53" s="37"/>
-      <c r="Y53" s="37"/>
-      <c r="Z53" s="37"/>
-      <c r="AA53" s="37"/>
-      <c r="AB53" s="37"/>
-      <c r="AC53" s="37"/>
-      <c r="AD53" s="37"/>
-      <c r="AE53" s="37"/>
-      <c r="AF53" s="38"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="50"/>
+      <c r="L53" s="50"/>
+      <c r="M53" s="50"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="50"/>
+      <c r="S53" s="50"/>
+      <c r="T53" s="50"/>
+      <c r="U53" s="50"/>
+      <c r="V53" s="50"/>
+      <c r="W53" s="50"/>
+      <c r="X53" s="50"/>
+      <c r="Y53" s="50"/>
+      <c r="Z53" s="50"/>
+      <c r="AA53" s="50"/>
+      <c r="AB53" s="50"/>
+      <c r="AC53" s="50"/>
+      <c r="AD53" s="50"/>
+      <c r="AE53" s="50"/>
+      <c r="AF53" s="51"/>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
@@ -3213,33 +3046,33 @@
       <c r="E54" s="10">
         <v>1</v>
       </c>
-      <c r="F54" s="36"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="41"/>
-      <c r="K54" s="41"/>
-      <c r="L54" s="41"/>
-      <c r="M54" s="41"/>
-      <c r="N54" s="41"/>
-      <c r="O54" s="41"/>
-      <c r="P54" s="37"/>
-      <c r="Q54" s="37"/>
-      <c r="R54" s="37"/>
-      <c r="S54" s="37"/>
-      <c r="T54" s="37"/>
-      <c r="U54" s="37"/>
-      <c r="V54" s="37"/>
-      <c r="W54" s="37"/>
-      <c r="X54" s="37"/>
-      <c r="Y54" s="37"/>
-      <c r="Z54" s="37"/>
-      <c r="AA54" s="37"/>
-      <c r="AB54" s="37"/>
-      <c r="AC54" s="37"/>
-      <c r="AD54" s="37"/>
-      <c r="AE54" s="37"/>
-      <c r="AF54" s="38"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="54"/>
+      <c r="K54" s="54"/>
+      <c r="L54" s="54"/>
+      <c r="M54" s="54"/>
+      <c r="N54" s="54"/>
+      <c r="O54" s="54"/>
+      <c r="P54" s="50"/>
+      <c r="Q54" s="50"/>
+      <c r="R54" s="50"/>
+      <c r="S54" s="50"/>
+      <c r="T54" s="50"/>
+      <c r="U54" s="50"/>
+      <c r="V54" s="50"/>
+      <c r="W54" s="50"/>
+      <c r="X54" s="50"/>
+      <c r="Y54" s="50"/>
+      <c r="Z54" s="50"/>
+      <c r="AA54" s="50"/>
+      <c r="AB54" s="50"/>
+      <c r="AC54" s="50"/>
+      <c r="AD54" s="50"/>
+      <c r="AE54" s="50"/>
+      <c r="AF54" s="51"/>
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
@@ -3254,33 +3087,33 @@
       <c r="E55" s="10">
         <v>3</v>
       </c>
-      <c r="F55" s="36"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="37"/>
-      <c r="L55" s="37"/>
-      <c r="M55" s="37"/>
-      <c r="N55" s="37"/>
-      <c r="O55" s="37"/>
-      <c r="P55" s="37"/>
-      <c r="Q55" s="37"/>
-      <c r="R55" s="37"/>
-      <c r="S55" s="37"/>
-      <c r="T55" s="37"/>
-      <c r="U55" s="37"/>
-      <c r="V55" s="37"/>
-      <c r="W55" s="37"/>
-      <c r="X55" s="37"/>
-      <c r="Y55" s="37"/>
-      <c r="Z55" s="37"/>
-      <c r="AA55" s="43"/>
-      <c r="AB55" s="37"/>
-      <c r="AC55" s="37"/>
-      <c r="AD55" s="37"/>
-      <c r="AE55" s="37"/>
-      <c r="AF55" s="38"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="50"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="50"/>
+      <c r="L55" s="50"/>
+      <c r="M55" s="50"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="50"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="50"/>
+      <c r="S55" s="50"/>
+      <c r="T55" s="50"/>
+      <c r="U55" s="50"/>
+      <c r="V55" s="50"/>
+      <c r="W55" s="50"/>
+      <c r="X55" s="50"/>
+      <c r="Y55" s="50"/>
+      <c r="Z55" s="50"/>
+      <c r="AA55" s="59"/>
+      <c r="AB55" s="50"/>
+      <c r="AC55" s="50"/>
+      <c r="AD55" s="50"/>
+      <c r="AE55" s="50"/>
+      <c r="AF55" s="51"/>
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
@@ -3295,33 +3128,33 @@
       <c r="E56" s="10">
         <v>4</v>
       </c>
-      <c r="F56" s="36"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="37"/>
-      <c r="M56" s="37"/>
-      <c r="N56" s="37"/>
-      <c r="O56" s="43"/>
-      <c r="P56" s="43"/>
-      <c r="Q56" s="43"/>
-      <c r="R56" s="43"/>
-      <c r="S56" s="43"/>
-      <c r="T56" s="43"/>
-      <c r="U56" s="43"/>
-      <c r="V56" s="43"/>
-      <c r="W56" s="37"/>
-      <c r="X56" s="37"/>
-      <c r="Y56" s="37"/>
-      <c r="Z56" s="37"/>
-      <c r="AA56" s="37"/>
-      <c r="AB56" s="37"/>
-      <c r="AC56" s="37"/>
-      <c r="AD56" s="37"/>
-      <c r="AE56" s="37"/>
-      <c r="AF56" s="38"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="50"/>
+      <c r="K56" s="50"/>
+      <c r="L56" s="50"/>
+      <c r="M56" s="50"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="59"/>
+      <c r="P56" s="59"/>
+      <c r="Q56" s="59"/>
+      <c r="R56" s="59"/>
+      <c r="S56" s="59"/>
+      <c r="T56" s="59"/>
+      <c r="U56" s="59"/>
+      <c r="V56" s="59"/>
+      <c r="W56" s="50"/>
+      <c r="X56" s="50"/>
+      <c r="Y56" s="50"/>
+      <c r="Z56" s="50"/>
+      <c r="AA56" s="50"/>
+      <c r="AB56" s="50"/>
+      <c r="AC56" s="50"/>
+      <c r="AD56" s="50"/>
+      <c r="AE56" s="50"/>
+      <c r="AF56" s="51"/>
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
@@ -3336,33 +3169,33 @@
       <c r="E57" s="10">
         <v>5</v>
       </c>
-      <c r="F57" s="36"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="37"/>
-      <c r="M57" s="37"/>
-      <c r="N57" s="37"/>
-      <c r="O57" s="37"/>
-      <c r="P57" s="37"/>
-      <c r="Q57" s="37"/>
-      <c r="R57" s="37"/>
-      <c r="S57" s="37"/>
-      <c r="T57" s="37"/>
-      <c r="U57" s="37"/>
-      <c r="V57" s="37"/>
-      <c r="W57" s="41"/>
-      <c r="X57" s="41"/>
-      <c r="Y57" s="41"/>
-      <c r="Z57" s="41"/>
-      <c r="AA57" s="37"/>
-      <c r="AB57" s="37"/>
-      <c r="AC57" s="37"/>
-      <c r="AD57" s="37"/>
-      <c r="AE57" s="37"/>
-      <c r="AF57" s="38"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="50"/>
+      <c r="K57" s="50"/>
+      <c r="L57" s="50"/>
+      <c r="M57" s="50"/>
+      <c r="N57" s="50"/>
+      <c r="O57" s="50"/>
+      <c r="P57" s="50"/>
+      <c r="Q57" s="50"/>
+      <c r="R57" s="50"/>
+      <c r="S57" s="50"/>
+      <c r="T57" s="50"/>
+      <c r="U57" s="50"/>
+      <c r="V57" s="50"/>
+      <c r="W57" s="54"/>
+      <c r="X57" s="54"/>
+      <c r="Y57" s="54"/>
+      <c r="Z57" s="54"/>
+      <c r="AA57" s="50"/>
+      <c r="AB57" s="50"/>
+      <c r="AC57" s="50"/>
+      <c r="AD57" s="50"/>
+      <c r="AE57" s="50"/>
+      <c r="AF57" s="51"/>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
@@ -3377,33 +3210,33 @@
       <c r="E58" s="10">
         <v>6</v>
       </c>
-      <c r="F58" s="42"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
-      <c r="L58" s="37"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="37"/>
-      <c r="O58" s="37"/>
-      <c r="P58" s="37"/>
-      <c r="Q58" s="37"/>
-      <c r="R58" s="37"/>
-      <c r="S58" s="37"/>
-      <c r="T58" s="37"/>
-      <c r="U58" s="37"/>
-      <c r="V58" s="37"/>
-      <c r="W58" s="37"/>
-      <c r="X58" s="37"/>
-      <c r="Y58" s="37"/>
-      <c r="Z58" s="37"/>
-      <c r="AA58" s="37"/>
-      <c r="AB58" s="37"/>
-      <c r="AC58" s="37"/>
-      <c r="AD58" s="37"/>
-      <c r="AE58" s="37"/>
-      <c r="AF58" s="38"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="50"/>
+      <c r="K58" s="50"/>
+      <c r="L58" s="50"/>
+      <c r="M58" s="50"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="50"/>
+      <c r="P58" s="50"/>
+      <c r="Q58" s="50"/>
+      <c r="R58" s="50"/>
+      <c r="S58" s="50"/>
+      <c r="T58" s="50"/>
+      <c r="U58" s="50"/>
+      <c r="V58" s="50"/>
+      <c r="W58" s="50"/>
+      <c r="X58" s="50"/>
+      <c r="Y58" s="50"/>
+      <c r="Z58" s="50"/>
+      <c r="AA58" s="50"/>
+      <c r="AB58" s="50"/>
+      <c r="AC58" s="50"/>
+      <c r="AD58" s="50"/>
+      <c r="AE58" s="50"/>
+      <c r="AF58" s="51"/>
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
@@ -3418,33 +3251,33 @@
       <c r="E59" s="10">
         <v>7</v>
       </c>
-      <c r="F59" s="36"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="41"/>
-      <c r="J59" s="41"/>
-      <c r="K59" s="41"/>
-      <c r="L59" s="41"/>
-      <c r="M59" s="41"/>
-      <c r="N59" s="41"/>
-      <c r="O59" s="37"/>
-      <c r="P59" s="37"/>
-      <c r="Q59" s="37"/>
-      <c r="R59" s="37"/>
-      <c r="S59" s="37"/>
-      <c r="T59" s="37"/>
-      <c r="U59" s="37"/>
-      <c r="V59" s="37"/>
-      <c r="W59" s="37"/>
-      <c r="X59" s="37"/>
-      <c r="Y59" s="37"/>
-      <c r="Z59" s="37"/>
-      <c r="AA59" s="37"/>
-      <c r="AB59" s="37"/>
-      <c r="AC59" s="37"/>
-      <c r="AD59" s="37"/>
-      <c r="AE59" s="37"/>
-      <c r="AF59" s="38"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
+      <c r="I59" s="54"/>
+      <c r="J59" s="54"/>
+      <c r="K59" s="54"/>
+      <c r="L59" s="54"/>
+      <c r="M59" s="54"/>
+      <c r="N59" s="54"/>
+      <c r="O59" s="50"/>
+      <c r="P59" s="50"/>
+      <c r="Q59" s="50"/>
+      <c r="R59" s="50"/>
+      <c r="S59" s="50"/>
+      <c r="T59" s="50"/>
+      <c r="U59" s="50"/>
+      <c r="V59" s="50"/>
+      <c r="W59" s="50"/>
+      <c r="X59" s="50"/>
+      <c r="Y59" s="50"/>
+      <c r="Z59" s="50"/>
+      <c r="AA59" s="50"/>
+      <c r="AB59" s="50"/>
+      <c r="AC59" s="50"/>
+      <c r="AD59" s="50"/>
+      <c r="AE59" s="50"/>
+      <c r="AF59" s="51"/>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
@@ -3459,33 +3292,33 @@
       <c r="E60" s="10">
         <v>9</v>
       </c>
-      <c r="F60" s="36"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="37"/>
-      <c r="L60" s="37"/>
-      <c r="M60" s="37"/>
-      <c r="N60" s="37"/>
-      <c r="O60" s="37"/>
-      <c r="P60" s="37"/>
-      <c r="Q60" s="37"/>
-      <c r="R60" s="37"/>
-      <c r="S60" s="37"/>
-      <c r="T60" s="37"/>
-      <c r="U60" s="37"/>
-      <c r="V60" s="37"/>
-      <c r="W60" s="37"/>
-      <c r="X60" s="41"/>
-      <c r="Y60" s="41"/>
-      <c r="Z60" s="37"/>
-      <c r="AA60" s="37"/>
-      <c r="AB60" s="37"/>
-      <c r="AC60" s="37"/>
-      <c r="AD60" s="37"/>
-      <c r="AE60" s="37"/>
-      <c r="AF60" s="38"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="50"/>
+      <c r="H60" s="50"/>
+      <c r="I60" s="50"/>
+      <c r="J60" s="50"/>
+      <c r="K60" s="50"/>
+      <c r="L60" s="50"/>
+      <c r="M60" s="50"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="50"/>
+      <c r="P60" s="50"/>
+      <c r="Q60" s="50"/>
+      <c r="R60" s="50"/>
+      <c r="S60" s="50"/>
+      <c r="T60" s="50"/>
+      <c r="U60" s="50"/>
+      <c r="V60" s="50"/>
+      <c r="W60" s="50"/>
+      <c r="X60" s="54"/>
+      <c r="Y60" s="54"/>
+      <c r="Z60" s="50"/>
+      <c r="AA60" s="50"/>
+      <c r="AB60" s="50"/>
+      <c r="AC60" s="50"/>
+      <c r="AD60" s="50"/>
+      <c r="AE60" s="50"/>
+      <c r="AF60" s="51"/>
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
@@ -3500,33 +3333,33 @@
       <c r="E61" s="10">
         <v>10</v>
       </c>
-      <c r="F61" s="36"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="41"/>
-      <c r="L61" s="41"/>
-      <c r="M61" s="41"/>
-      <c r="N61" s="41"/>
-      <c r="O61" s="41"/>
-      <c r="P61" s="41"/>
-      <c r="Q61" s="37"/>
-      <c r="R61" s="37"/>
-      <c r="S61" s="37"/>
-      <c r="T61" s="37"/>
-      <c r="U61" s="37"/>
-      <c r="V61" s="37"/>
-      <c r="W61" s="37"/>
-      <c r="X61" s="37"/>
-      <c r="Y61" s="37"/>
-      <c r="Z61" s="37"/>
-      <c r="AA61" s="37"/>
-      <c r="AB61" s="37"/>
-      <c r="AC61" s="37"/>
-      <c r="AD61" s="37"/>
-      <c r="AE61" s="37"/>
-      <c r="AF61" s="38"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="54"/>
+      <c r="L61" s="54"/>
+      <c r="M61" s="54"/>
+      <c r="N61" s="54"/>
+      <c r="O61" s="54"/>
+      <c r="P61" s="54"/>
+      <c r="Q61" s="50"/>
+      <c r="R61" s="50"/>
+      <c r="S61" s="50"/>
+      <c r="T61" s="50"/>
+      <c r="U61" s="50"/>
+      <c r="V61" s="50"/>
+      <c r="W61" s="50"/>
+      <c r="X61" s="50"/>
+      <c r="Y61" s="50"/>
+      <c r="Z61" s="50"/>
+      <c r="AA61" s="50"/>
+      <c r="AB61" s="50"/>
+      <c r="AC61" s="50"/>
+      <c r="AD61" s="50"/>
+      <c r="AE61" s="50"/>
+      <c r="AF61" s="51"/>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
@@ -3541,33 +3374,33 @@
       <c r="E62" s="10">
         <v>11</v>
       </c>
-      <c r="F62" s="36"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="37"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="37"/>
-      <c r="P62" s="37"/>
-      <c r="Q62" s="41"/>
-      <c r="R62" s="41"/>
-      <c r="S62" s="41"/>
-      <c r="T62" s="41"/>
-      <c r="U62" s="41"/>
-      <c r="V62" s="41"/>
-      <c r="W62" s="41"/>
-      <c r="X62" s="37"/>
-      <c r="Y62" s="37"/>
-      <c r="Z62" s="37"/>
-      <c r="AA62" s="37"/>
-      <c r="AB62" s="37"/>
-      <c r="AC62" s="37"/>
-      <c r="AD62" s="37"/>
-      <c r="AE62" s="37"/>
-      <c r="AF62" s="38"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="50"/>
+      <c r="H62" s="50"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="50"/>
+      <c r="K62" s="50"/>
+      <c r="L62" s="50"/>
+      <c r="M62" s="50"/>
+      <c r="N62" s="50"/>
+      <c r="O62" s="50"/>
+      <c r="P62" s="50"/>
+      <c r="Q62" s="54"/>
+      <c r="R62" s="54"/>
+      <c r="S62" s="54"/>
+      <c r="T62" s="54"/>
+      <c r="U62" s="54"/>
+      <c r="V62" s="54"/>
+      <c r="W62" s="54"/>
+      <c r="X62" s="50"/>
+      <c r="Y62" s="50"/>
+      <c r="Z62" s="50"/>
+      <c r="AA62" s="50"/>
+      <c r="AB62" s="50"/>
+      <c r="AC62" s="50"/>
+      <c r="AD62" s="50"/>
+      <c r="AE62" s="50"/>
+      <c r="AF62" s="51"/>
     </row>
     <row r="63" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="21" t="s">

</xml_diff>